<commit_message>
Adding latest code for "Ont This Page" section
</commit_message>
<xml_diff>
--- a/test-data/on-this-page-data.xlsx
+++ b/test-data/on-this-page-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FAEDCC-362C-F740-AABA-8A7D530418FF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD76022F-963F-234C-9CA1-6A893F1C5D3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10980" yWindow="1220" windowWidth="26280" windowHeight="18200" activeTab="1" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="420" yWindow="460" windowWidth="26280" windowHeight="13500" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_on_this_page" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>path</t>
   </si>
@@ -43,37 +43,16 @@
     <t>English</t>
   </si>
   <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>PDQ Cancer</t>
-  </si>
-  <si>
     <t>about-cancer/coping/self-image</t>
   </si>
   <si>
-    <t>header</t>
-  </si>
-  <si>
     <t>ON THIS PAGE</t>
   </si>
   <si>
-    <t>espanol/cancer/sobrellevar/self-image</t>
-  </si>
-  <si>
-    <t>EN ESTA PÁGINA</t>
-  </si>
-  <si>
-    <t>espanol/cancer/tratamiento/mca/paciente/cartilago-pdq</t>
-  </si>
-  <si>
-    <t>about-cancer/treatment/cam/patient/cartilage-pdq</t>
-  </si>
-  <si>
-    <t>types/breast/reconstruction-fact-sheet</t>
-  </si>
-  <si>
     <t>about-cancer/coping/feelings/relaxation</t>
+  </si>
+  <si>
+    <t>otpHeader</t>
   </si>
 </sst>
 </file>
@@ -435,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E50E58-C20E-6840-B475-2B9A8D9E132C}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="69.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.83203125" customWidth="1"/>
@@ -465,7 +444,7 @@
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -474,63 +453,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -542,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B4152C-D020-1F46-B7E3-749FB40F63A8}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,7 +489,7 @@
     </row>
     <row r="2" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Pushing the latest code changes for "On This Page" section
</commit_message>
<xml_diff>
--- a/test-data/on-this-page-data.xlsx
+++ b/test-data/on-this-page-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/popkhadzeg/eclipse-workspace/cgov-digital-platform-qa/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD76022F-963F-234C-9CA1-6A893F1C5D3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAE1AB4-5D00-1F40-8F84-B76000F74AB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="460" windowWidth="26280" windowHeight="13500" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
+    <workbookView xWindow="2680" yWindow="1240" windowWidth="26280" windowHeight="13500" xr2:uid="{150E7FB9-AAC7-684F-9B42-02331F762CE7}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_on_this_page" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>path</t>
   </si>
@@ -53,6 +53,45 @@
   </si>
   <si>
     <t>otpHeader</t>
+  </si>
+  <si>
+    <t>espanol/cancer/sobrellevar/self-image</t>
+  </si>
+  <si>
+    <t>EN ESTA PÁGINA</t>
+  </si>
+  <si>
+    <t>types/lung/patient/lung-prevention-pdq</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>espanol/tipos/pulmon/paciente/prevencion-pulmon-pdq</t>
+  </si>
+  <si>
+    <t>PDQ Cancer Info</t>
+  </si>
+  <si>
+    <t>news-events/press-releases/2018/brca-exchange-test</t>
+  </si>
+  <si>
+    <t>espanol/tipos/seno</t>
+  </si>
+  <si>
+    <t>Cancer Type Homepage</t>
+  </si>
+  <si>
+    <t>Press Release</t>
+  </si>
+  <si>
+    <t>Blog</t>
+  </si>
+  <si>
+    <t>espanol/news-events/cancer-currents-blog/2019/vitamina-d-complemento-cancer-prevencion</t>
+  </si>
+  <si>
+    <t>espanol/cancer/sobrellevar/placeholder-men</t>
   </si>
 </sst>
 </file>
@@ -96,10 +135,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41E50E58-C20E-6840-B475-2B9A8D9E132C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,6 +496,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -463,16 +545,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B4152C-D020-1F46-B7E3-749FB40F63A8}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="69.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -498,6 +580,50 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>